<commit_message>
Alterações no Product backlog e GANTT
</commit_message>
<xml_diff>
--- a/SPRINT2/Gráfico de GANTT.xlsx
+++ b/SPRINT2/Gráfico de GANTT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facul\PROJETO PI DREAM HOUSE\Documentação do projeto\Documentos\SPRINT2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\SPRINT2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722AED14-D136-4801-A899-12405F8AED9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58952B11-E128-4B90-824E-CDA2256D9C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="461" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="461" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MODELO" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>#</t>
   </si>
@@ -55,27 +55,6 @@
   </si>
   <si>
     <t>%</t>
-  </si>
-  <si>
-    <t>Reunião com o cliente</t>
-  </si>
-  <si>
-    <t>Definição do escopo</t>
-  </si>
-  <si>
-    <t>Aprovação do cliente</t>
-  </si>
-  <si>
-    <t>Aprovação na prefeitura</t>
-  </si>
-  <si>
-    <t>Finalização do projeto executivo</t>
-  </si>
-  <si>
-    <t>Entrega para o cliente</t>
-  </si>
-  <si>
-    <t>Elaboração dos projetos</t>
   </si>
   <si>
     <t>Data Atual</t>
@@ -566,11 +545,11 @@
     <xf numFmtId="14" fontId="9" fillId="8" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="8" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -584,7 +563,28 @@
     <cellStyle name="Ruim" xfId="3" builtinId="27"/>
     <cellStyle name="Saída" xfId="5" builtinId="21"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -949,7 +949,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.2631578947368418E-2</c:v>
+                  <c:v>0.10526315789473684</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2015,7 +2015,7 @@
       <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2360,7 +2360,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D3" s="11">
         <v>1</v>
@@ -2437,7 +2437,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" s="7">
         <v>2</v>
@@ -2446,7 +2446,7 @@
         <v>42493</v>
       </c>
       <c r="F4" s="9">
-        <f t="shared" ref="F4:F9" si="1">WORKDAY(E4,(D4-1))</f>
+        <f t="shared" ref="F4:F10" si="1">WORKDAY(E4,(D4-1))</f>
         <v>42494</v>
       </c>
       <c r="G4" s="10">
@@ -2514,7 +2514,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="7">
         <v>15</v>
@@ -2591,7 +2591,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D6" s="7">
         <v>1</v>
@@ -2668,7 +2668,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D7" s="7">
         <v>30</v>
@@ -2745,7 +2745,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D8" s="7">
         <v>10</v>
@@ -2822,7 +2822,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
@@ -2898,11 +2898,22 @@
       <c r="B10" s="7">
         <v>8</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="10"/>
+      <c r="C10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="7">
+        <v>2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>44663</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" si="1"/>
+        <v>44664</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
       <c r="H10" s="21"/>
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
@@ -2980,13 +2991,28 @@
     <mergeCell ref="AC1:AI1"/>
     <mergeCell ref="AJ1:AP1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:G10">
-    <cfRule type="expression" dxfId="21" priority="2">
+  <conditionalFormatting sqref="B3:B10 D3:G9 D10 G10">
+    <cfRule type="expression" dxfId="24" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:BK10">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="23" priority="4">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C9">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:F10">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3000,10 +3026,10 @@
   <dimension ref="A1:EQ24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="8" topLeftCell="H9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="8" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4:E4"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3019,7 +3045,7 @@
   <sheetData>
     <row r="1" spans="1:147" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -3038,8 +3064,8 @@
       <c r="G2" s="31"/>
     </row>
     <row r="4" spans="1:147" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="38" t="s">
-        <v>15</v>
+      <c r="C4" s="37" t="s">
+        <v>8</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>3</v>
@@ -3051,31 +3077,31 @@
       <c r="G4" s="35"/>
     </row>
     <row r="5" spans="1:147" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="38"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="33" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E5" s="33"/>
       <c r="F5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44648</v>
+        <v>44654</v>
       </c>
       <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:147" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="27">
         <f>(SUM(CÁLCULOS!A3:A22)/SUM('COM FÓRMULAS'!D9:D20))</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0.10526315789473684</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E6" s="34"/>
-      <c r="F6" s="37">
+      <c r="F6" s="38">
         <f>(F20-E9)+1</f>
         <v>25</v>
       </c>
-      <c r="G6" s="37"/>
+      <c r="G6" s="38"/>
     </row>
     <row r="7" spans="1:147" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H7" s="28">
@@ -3865,7 +3891,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D9" s="25">
         <v>1</v>
@@ -4026,7 +4052,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D10" s="26">
         <v>1</v>
@@ -4039,7 +4065,7 @@
         <v>44648</v>
       </c>
       <c r="G10" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
@@ -4187,7 +4213,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D11" s="26">
         <v>2</v>
@@ -4348,7 +4374,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D12" s="26">
         <v>1</v>
@@ -4509,7 +4535,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D13" s="26">
         <v>2</v>
@@ -4670,7 +4696,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D14" s="26">
         <v>2</v>
@@ -4831,7 +4857,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D15" s="26">
         <v>2</v>
@@ -4992,7 +5018,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D16" s="26">
         <v>2</v>
@@ -5153,7 +5179,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D17" s="26">
         <v>2</v>
@@ -5314,7 +5340,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D18" s="26">
         <v>1</v>
@@ -5475,7 +5501,7 @@
         <v>11</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D19" s="26">
         <v>1</v>
@@ -5636,7 +5662,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D20" s="26">
         <v>2</v>
@@ -5799,6 +5825,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="EK7:EQ7"/>
+    <mergeCell ref="BE7:BK7"/>
+    <mergeCell ref="BS7:BY7"/>
+    <mergeCell ref="BZ7:CF7"/>
+    <mergeCell ref="CG7:CM7"/>
+    <mergeCell ref="CN7:CT7"/>
+    <mergeCell ref="CU7:DA7"/>
+    <mergeCell ref="DB7:DH7"/>
+    <mergeCell ref="DI7:DO7"/>
+    <mergeCell ref="DP7:DV7"/>
+    <mergeCell ref="DW7:EC7"/>
+    <mergeCell ref="ED7:EJ7"/>
     <mergeCell ref="AX7:BD7"/>
     <mergeCell ref="BL7:BR7"/>
     <mergeCell ref="A1:G2"/>
@@ -5815,51 +5853,39 @@
     <mergeCell ref="AC7:AI7"/>
     <mergeCell ref="AJ7:AP7"/>
     <mergeCell ref="AQ7:AW7"/>
-    <mergeCell ref="EK7:EQ7"/>
-    <mergeCell ref="BE7:BK7"/>
-    <mergeCell ref="BS7:BY7"/>
-    <mergeCell ref="BZ7:CF7"/>
-    <mergeCell ref="CG7:CM7"/>
-    <mergeCell ref="CN7:CT7"/>
-    <mergeCell ref="CU7:DA7"/>
-    <mergeCell ref="DB7:DH7"/>
-    <mergeCell ref="DI7:DO7"/>
-    <mergeCell ref="DP7:DV7"/>
-    <mergeCell ref="DW7:EC7"/>
-    <mergeCell ref="ED7:EJ7"/>
   </mergeCells>
   <conditionalFormatting sqref="B18:D19 B17 D17 B9:G10 B16:D16 E16:F20 B11:F15 G11:G20">
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="22" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:BD19 BL9:EQ19">
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="21" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:BD19 BL9:EQ19">
-    <cfRule type="expression" dxfId="17" priority="17">
+    <cfRule type="expression" dxfId="20" priority="17">
       <formula>AND(H$8&gt;=$E9,H$8&lt;=$F9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:BD19 BL9:EQ19">
-    <cfRule type="expression" dxfId="16" priority="18">
+    <cfRule type="expression" dxfId="19" priority="18">
       <formula>OR(WEEKDAY(H$8,2)=6,WEEKDAY(H$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE9:BK19">
-    <cfRule type="expression" dxfId="15" priority="15">
+    <cfRule type="expression" dxfId="18" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE9:BK19">
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="17" priority="13">
       <formula>AND(BE$8&gt;=$E9,BE$8&lt;=$F9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE9:BK19">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="16" priority="14">
       <formula>OR(WEEKDAY(BE$8,2)=6,WEEKDAY(BE$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5878,42 +5904,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:D20">
-    <cfRule type="expression" dxfId="12" priority="10">
+    <cfRule type="expression" dxfId="15" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20:BD20 BL20:EQ20">
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="14" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20:BD20 BL20:EQ20">
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="13" priority="7">
       <formula>AND(H$8&gt;=$E20,H$8&lt;=$F20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20:BD20 BL20:EQ20">
-    <cfRule type="expression" dxfId="9" priority="8">
+    <cfRule type="expression" dxfId="12" priority="8">
       <formula>OR(WEEKDAY(H$8,2)=6,WEEKDAY(H$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE20:BK20">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE20:BK20">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>AND(BE$8&gt;=$E20,BE$8&lt;=$F20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE20:BK20">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="9" priority="4">
       <formula>OR(WEEKDAY(BE$8,2)=6,WEEKDAY(BE$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6014,7 +6040,7 @@
   <dimension ref="A3:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6035,11 +6061,11 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>'COM FÓRMULAS'!D10*'COM FÓRMULAS'!G10</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" s="23">
         <f>IFERROR(WORKDAY('COM FÓRMULAS'!E10,CÁLCULOS!A4-1),"-")</f>
-        <v>44645</v>
+        <v>44648</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>